<commit_message>
Add data for Zi En Appointment & Doctor Availability
</commit_message>
<xml_diff>
--- a/data/Patient_List.xlsx
+++ b/data/Patient_List.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Patient ID</t>
   </si>
@@ -83,12 +83,16 @@
   </si>
   <si>
     <t>charlie.white@example.com</t>
+  </si>
+  <si>
+    <t>81234567</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -139,19 +143,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -160,10 +164,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -319,7 +323,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -328,13 +332,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -344,7 +348,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -353,7 +357,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -362,7 +366,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -372,12 +376,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -408,7 +412,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -427,7 +431,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -440,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -527,6 +531,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Appointment functionality, Load appointment, availability list, updated the patient, file paths, doctor functionality.
</commit_message>
<xml_diff>
--- a/data/Patient_List.xlsx
+++ b/data/Patient_List.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zent-zaxux/IdeaProjects/SC2002/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2F9CEA-3BB5-0C46-894A-071129E87163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="6180" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Patient ID</t>
   </si>
@@ -83,13 +89,31 @@
   </si>
   <si>
     <t>charlie.white@example.com</t>
+  </si>
+  <si>
+    <t>Doctor Diagnosis</t>
+  </si>
+  <si>
+    <t>Treatment Plan</t>
+  </si>
+  <si>
+    <t>require further followup, require medicine</t>
+  </si>
+  <si>
+    <t>followup, done</t>
+  </si>
+  <si>
+    <t>okay, not okay</t>
+  </si>
+  <si>
+    <t>nil, nil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,13 +176,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -196,7 +228,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -230,6 +262,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -264,9 +297,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -439,14 +473,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="25.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +504,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -485,8 +530,14 @@
       <c r="F2" t="s">
         <v>20</v>
       </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -505,8 +556,14 @@
       <c r="F3" t="s">
         <v>21</v>
       </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
update patient to have both phone number and email
</commit_message>
<xml_diff>
--- a/data/Patient_List.xlsx
+++ b/data/Patient_List.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zent-zaxux/IdeaProjects/SC2002/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hx/Documents/SC2002/OOP_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{B868F784-081D-0A46-B0E6-55561003E6F9}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EC4440-E22C-BF4F-83B2-16FF45C2E8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15820" windowWidth="22060" xWindow="6180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="500"/>
+    <workbookView xWindow="6180" yWindow="760" windowWidth="22060" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Patient ID</t>
   </si>
@@ -110,13 +110,15 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -167,19 +169,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -196,10 +202,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -357,7 +363,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -366,13 +372,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -382,7 +388,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -391,7 +397,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -400,7 +406,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -410,12 +416,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -446,7 +452,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -465,7 +471,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -477,20 +483,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="144">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="11.33203125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,8 +524,11 @@
       <c r="H1" t="s">
         <v>24</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -541,8 +553,11 @@
       <c r="H2" t="s">
         <v>28</v>
       </c>
+      <c r="I2" s="3">
+        <v>81234567</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -567,8 +582,11 @@
       <c r="H3" t="s">
         <v>26</v>
       </c>
+      <c r="I3" s="3">
+        <v>81112222</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -593,8 +611,11 @@
       <c r="H4" t="s">
         <v>29</v>
       </c>
+      <c r="I4" s="3">
+        <v>91234567</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>